<commit_message>
updated data dictionary after meeting 11/3
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Floorsweeper\Documents\CS\451\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Floorsweeper\Documents\GitHub\CMSC_451_Senior\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="731">
   <si>
     <t>Agriculture</t>
   </si>
@@ -736,9 +736,6 @@
     <t>Canal, irrigation</t>
   </si>
   <si>
-    <t>Employer/Contractor</t>
-  </si>
-  <si>
     <t>Fireplace, natural gas, installation</t>
   </si>
   <si>
@@ -1211,9 +1208,6 @@
   </si>
   <si>
     <t>Landscaping Service</t>
-  </si>
-  <si>
-    <t>Set Asides</t>
   </si>
   <si>
     <t>Toilet preparation manufacturing</t>
@@ -2043,141 +2037,204 @@
 We look forward to working with you in the future.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a new job listing, &lt;&lt;Job Name&gt;&gt; from &lt;&lt;Business Name&gt;&gt; that may be of interest. Please review the details at &lt;&lt;Job Link&gt;&gt;. </t>
+  </si>
+  <si>
+    <t>Message Body</t>
+  </si>
+  <si>
+    <t>Dear &lt;&lt;Representative Name&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Dear &lt;&lt;Vendor Manager Name&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Dear ???</t>
+  </si>
+  <si>
+    <t>Dear &lt;&lt;Vendor Manager Name&gt;&gt;,</t>
+  </si>
+  <si>
+    <t>To Whom It May Concern,</t>
+  </si>
+  <si>
+    <t>Dear &lt;&lt;Representative Name&gt;&gt;,</t>
+  </si>
+  <si>
+    <t>Salutation</t>
+  </si>
+  <si>
+    <t>V05: Vendor profile successful</t>
+  </si>
+  <si>
+    <t>V04: More information for profile required</t>
+  </si>
+  <si>
+    <t>V03: Vendor profile rejected</t>
+  </si>
+  <si>
+    <t>V02: Vendor profile created (To VM)</t>
+  </si>
+  <si>
+    <t>V01: Vendor profile created (To vendor)</t>
+  </si>
+  <si>
+    <t>JA05: Job application denied</t>
+  </si>
+  <si>
+    <t>JA04: Vendor manager relaying information to business</t>
+  </si>
+  <si>
+    <t>JA03: Vendor application</t>
+  </si>
+  <si>
+    <t>JA02: Vendor inquiry about job posting</t>
+  </si>
+  <si>
+    <t>JA01: Business posts job</t>
+  </si>
+  <si>
+    <t>Notification Name</t>
+  </si>
+  <si>
+    <t>SLA#</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Begins</t>
+  </si>
+  <si>
+    <t>Start Condition</t>
+  </si>
+  <si>
+    <t>Stop Condition</t>
+  </si>
+  <si>
+    <t>Ends</t>
+  </si>
+  <si>
+    <t>Pause Condition</t>
+  </si>
+  <si>
+    <t>Penalty</t>
+  </si>
+  <si>
+    <t>Profile Review</t>
+  </si>
+  <si>
+    <t>48 Hr</t>
+  </si>
+  <si>
+    <t>Profile Addendum</t>
+  </si>
+  <si>
+    <t>Job App Review</t>
+  </si>
+  <si>
+    <t>72 Hr</t>
+  </si>
+  <si>
+    <t>Job 5</t>
+  </si>
+  <si>
+    <t>Job 6</t>
+  </si>
+  <si>
+    <t>Job 8.3</t>
+  </si>
+  <si>
+    <t>Profile 3</t>
+  </si>
+  <si>
+    <t>Profile 7.1</t>
+  </si>
+  <si>
+    <t>Profile 4</t>
+  </si>
+  <si>
+    <t>Profile 7.2</t>
+  </si>
+  <si>
+    <t>Profile 7</t>
+  </si>
+  <si>
+    <t>Profile 7.3</t>
+  </si>
+  <si>
+    <t>Client name</t>
+  </si>
+  <si>
+    <t>Business Classifications/Set Asides</t>
+  </si>
+  <si>
+    <t>Veteran Owned Business</t>
+  </si>
+  <si>
+    <t>Small Business</t>
+  </si>
+  <si>
+    <t>Economically-Disadvantaged Women-Owned Small Business (EDWOSB)</t>
+  </si>
+  <si>
+    <t>An HBCU or Minority Institution</t>
+  </si>
+  <si>
+    <t>Federally Recognized Tribal Business or Alaska Corporation</t>
+  </si>
+  <si>
+    <t>State Recognized Tribal Business</t>
+  </si>
+  <si>
+    <t>8(a) Business</t>
+  </si>
+  <si>
+    <t>American Indian Owner</t>
+  </si>
+  <si>
+    <t>Alaska Native Owner </t>
+  </si>
+  <si>
+    <t>Type of Business</t>
+  </si>
+  <si>
+    <t>Corporation</t>
+  </si>
+  <si>
+    <t>Educational Institution</t>
+  </si>
+  <si>
+    <t>LLC</t>
+  </si>
+  <si>
+    <t>LLP</t>
+  </si>
+  <si>
+    <t>NPO</t>
+  </si>
+  <si>
+    <t>Partnership</t>
+  </si>
+  <si>
+    <t>Sole Proprietor</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Doing Business As</t>
+  </si>
+  <si>
     <t>We have reviewed the job, &lt;&lt;Job Name&gt;&gt;, and have inquiries regarding the listing. The questions/comments are as follows: 
-&lt;&lt;USER EDIT&gt;&gt;
+&lt;&lt;User Edit&gt;&gt;
 We look forward to your response.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a new job listing, &lt;&lt;Job Name&gt;&gt; from &lt;&lt;Business Name&gt;&gt; that may be of interest. Please review the details at &lt;&lt;Job Link&gt;&gt;. </t>
-  </si>
-  <si>
-    <t>Message Body</t>
-  </si>
-  <si>
-    <t>Dear &lt;&lt;Representative Name&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Dear &lt;&lt;Vendor Manager Name&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Dear ???</t>
-  </si>
-  <si>
-    <t>Dear &lt;&lt;Vendor Manager Name&gt;&gt;,</t>
-  </si>
-  <si>
-    <t>To Whom It May Concern,</t>
-  </si>
-  <si>
-    <t>Dear &lt;&lt;Representative Name&gt;&gt;,</t>
-  </si>
-  <si>
-    <t>Salutation</t>
-  </si>
-  <si>
-    <t>V05: Vendor profile successful</t>
-  </si>
-  <si>
-    <t>V04: More information for profile required</t>
-  </si>
-  <si>
-    <t>V03: Vendor profile rejected</t>
-  </si>
-  <si>
-    <t>V02: Vendor profile created (To VM)</t>
-  </si>
-  <si>
-    <t>V01: Vendor profile created (To vendor)</t>
-  </si>
-  <si>
-    <t>JA05: Job application denied</t>
-  </si>
-  <si>
-    <t>JA04: Vendor manager relaying information to business</t>
-  </si>
-  <si>
-    <t>JA03: Vendor application</t>
-  </si>
-  <si>
-    <t>JA02: Vendor inquiry about job posting</t>
-  </si>
-  <si>
-    <t>JA01: Business posts job</t>
-  </si>
-  <si>
-    <t>Notification Name</t>
-  </si>
-  <si>
-    <t>SLA#</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Schedule</t>
-  </si>
-  <si>
-    <t>Begins</t>
-  </si>
-  <si>
-    <t>Start Condition</t>
-  </si>
-  <si>
-    <t>Stop Condition</t>
-  </si>
-  <si>
-    <t>Ends</t>
-  </si>
-  <si>
-    <t>Pause Condition</t>
-  </si>
-  <si>
-    <t>Penalty</t>
-  </si>
-  <si>
-    <t>Profile Review</t>
-  </si>
-  <si>
-    <t>48 Hr</t>
-  </si>
-  <si>
-    <t>Profile Addendum</t>
-  </si>
-  <si>
-    <t>Job App Review</t>
-  </si>
-  <si>
-    <t>72 Hr</t>
-  </si>
-  <si>
-    <t>Job 5</t>
-  </si>
-  <si>
-    <t>Job 6</t>
-  </si>
-  <si>
-    <t>Job 8.3</t>
-  </si>
-  <si>
-    <t>Profile 3</t>
-  </si>
-  <si>
-    <t>Profile 7.1</t>
-  </si>
-  <si>
-    <t>Profile 4</t>
-  </si>
-  <si>
-    <t>Profile 7.2</t>
-  </si>
-  <si>
-    <t>Profile 7</t>
-  </si>
-  <si>
-    <t>Profile 7.3</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2404,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2377,34 +2453,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2549,6 +2597,34 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3101,13 +3177,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1190625</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -3176,13 +3252,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1457325</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -3253,53 +3329,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I22" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:I22"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Basic Information" dataDxfId="47"/>
-    <tableColumn id="2" name="Address" dataDxfId="46"/>
-    <tableColumn id="3" name="Sector" dataDxfId="45"/>
-    <tableColumn id="4" name="Revenue" dataDxfId="44"/>
-    <tableColumn id="5" name="Number of Employees" dataDxfId="43"/>
-    <tableColumn id="6" name="Vendor Experience" dataDxfId="42"/>
-    <tableColumn id="7" name="Industry" dataDxfId="41"/>
-    <tableColumn id="8" name="Set Asides" dataDxfId="40"/>
-    <tableColumn id="9" name="Skills" dataDxfId="39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J36" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+  <autoFilter ref="A1:J36"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Basic Information" dataDxfId="48"/>
+    <tableColumn id="2" name="Address" dataDxfId="47"/>
+    <tableColumn id="3" name="Sector" dataDxfId="46"/>
+    <tableColumn id="10" name="Type of Business" dataDxfId="0"/>
+    <tableColumn id="4" name="Revenue" dataDxfId="45"/>
+    <tableColumn id="5" name="Number of Employees" dataDxfId="44"/>
+    <tableColumn id="6" name="Vendor Experience" dataDxfId="43"/>
+    <tableColumn id="7" name="Industry" dataDxfId="42"/>
+    <tableColumn id="8" name="Business Classifications/Set Asides" dataDxfId="41"/>
+    <tableColumn id="9" name="Skills" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S175" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S175" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:S175"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="Agriculture" dataDxfId="36"/>
-    <tableColumn id="2" name="Utilities" dataDxfId="35"/>
-    <tableColumn id="3" name="Mining" dataDxfId="34"/>
-    <tableColumn id="4" name="Construction" dataDxfId="33"/>
-    <tableColumn id="5" name="Manufacturing" dataDxfId="32"/>
-    <tableColumn id="6" name="Information" dataDxfId="31"/>
-    <tableColumn id="7" name="Real Estate Rental and Leasing" dataDxfId="30"/>
-    <tableColumn id="8" name="Finance and Insurance" dataDxfId="29"/>
-    <tableColumn id="9" name="Retail Trade" dataDxfId="28"/>
-    <tableColumn id="10" name="Transportation and Warehousing" dataDxfId="27"/>
-    <tableColumn id="11" name="Professional, Scientific, and Technical Services" dataDxfId="26"/>
-    <tableColumn id="12" name="Management of Companies and Enterprises" dataDxfId="25"/>
-    <tableColumn id="13" name="Administrative and Support and Waste Management and Remediation Services" dataDxfId="24"/>
-    <tableColumn id="14" name="Educational Services" dataDxfId="23"/>
-    <tableColumn id="15" name="Health Care and Social Assistance" dataDxfId="22"/>
-    <tableColumn id="16" name="Arts, Entertainment, and Recreation" dataDxfId="21"/>
-    <tableColumn id="17" name="Accommodation and Food Services" dataDxfId="20"/>
-    <tableColumn id="18" name="Other Services (except Public Administration)" dataDxfId="19"/>
-    <tableColumn id="19" name="Public Administration" dataDxfId="18"/>
+    <tableColumn id="1" name="Agriculture" dataDxfId="37"/>
+    <tableColumn id="2" name="Utilities" dataDxfId="36"/>
+    <tableColumn id="3" name="Mining" dataDxfId="35"/>
+    <tableColumn id="4" name="Construction" dataDxfId="34"/>
+    <tableColumn id="5" name="Manufacturing" dataDxfId="33"/>
+    <tableColumn id="6" name="Information" dataDxfId="32"/>
+    <tableColumn id="7" name="Real Estate Rental and Leasing" dataDxfId="31"/>
+    <tableColumn id="8" name="Finance and Insurance" dataDxfId="30"/>
+    <tableColumn id="9" name="Retail Trade" dataDxfId="29"/>
+    <tableColumn id="10" name="Transportation and Warehousing" dataDxfId="28"/>
+    <tableColumn id="11" name="Professional, Scientific, and Technical Services" dataDxfId="27"/>
+    <tableColumn id="12" name="Management of Companies and Enterprises" dataDxfId="26"/>
+    <tableColumn id="13" name="Administrative and Support and Waste Management and Remediation Services" dataDxfId="25"/>
+    <tableColumn id="14" name="Educational Services" dataDxfId="24"/>
+    <tableColumn id="15" name="Health Care and Social Assistance" dataDxfId="23"/>
+    <tableColumn id="16" name="Arts, Entertainment, and Recreation" dataDxfId="22"/>
+    <tableColumn id="17" name="Accommodation and Food Services" dataDxfId="21"/>
+    <tableColumn id="18" name="Other Services (except Public Administration)" dataDxfId="20"/>
+    <tableColumn id="19" name="Public Administration" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:K5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:K5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:K5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3314,17 +3391,17 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" name="Notification Name" dataDxfId="17"/>
-    <tableColumn id="2" name="JA01: Business posts job" dataDxfId="16"/>
-    <tableColumn id="3" name="JA02: Vendor inquiry about job posting" dataDxfId="15"/>
-    <tableColumn id="4" name="JA03: Vendor application" dataDxfId="14"/>
-    <tableColumn id="5" name="JA04: Vendor manager relaying information to business" dataDxfId="13"/>
-    <tableColumn id="6" name="JA05: Job application denied" dataDxfId="12"/>
-    <tableColumn id="7" name="V01: Vendor profile created (To vendor)" dataDxfId="11"/>
-    <tableColumn id="8" name="V02: Vendor profile created (To VM)" dataDxfId="10"/>
-    <tableColumn id="9" name="V03: Vendor profile rejected" dataDxfId="9"/>
-    <tableColumn id="10" name="V04: More information for profile required" dataDxfId="8"/>
-    <tableColumn id="11" name="V05: Vendor profile successful" dataDxfId="7"/>
+    <tableColumn id="1" name="Notification Name" dataDxfId="16"/>
+    <tableColumn id="2" name="JA01: Business posts job" dataDxfId="15"/>
+    <tableColumn id="3" name="JA02: Vendor inquiry about job posting" dataDxfId="14"/>
+    <tableColumn id="4" name="JA03: Vendor application" dataDxfId="13"/>
+    <tableColumn id="5" name="JA04: Vendor manager relaying information to business" dataDxfId="12"/>
+    <tableColumn id="6" name="JA05: Job application denied" dataDxfId="11"/>
+    <tableColumn id="7" name="V01: Vendor profile created (To vendor)" dataDxfId="10"/>
+    <tableColumn id="8" name="V02: Vendor profile created (To VM)" dataDxfId="9"/>
+    <tableColumn id="9" name="V03: Vendor profile rejected" dataDxfId="8"/>
+    <tableColumn id="10" name="V04: More information for profile required" dataDxfId="7"/>
+    <tableColumn id="11" name="V05: Vendor profile successful" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3333,11 +3410,11 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E10" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" dataDxfId="4"/>
-    <tableColumn id="12" name="Column12" dataDxfId="3"/>
-    <tableColumn id="2" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" name="Column4" dataDxfId="0"/>
+    <tableColumn id="1" name="Column1" dataDxfId="5"/>
+    <tableColumn id="12" name="Column12" dataDxfId="4"/>
+    <tableColumn id="2" name="Column2" dataDxfId="3"/>
+    <tableColumn id="3" name="Column3" dataDxfId="2"/>
+    <tableColumn id="4" name="Column4" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3640,10 +3717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3651,393 +3728,453 @@
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>206</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>720</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>641</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>282</v>
+        <v>647</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>396</v>
+        <v>281</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>710</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>215</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>642</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>237</v>
+        <v>640</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>291</v>
+        <v>709</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>401</v>
+        <v>290</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>221</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>643</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>248</v>
+        <v>641</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I3" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>229</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>644</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>257</v>
+        <v>642</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I4" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>234</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>645</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I5" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>646</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>647</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>648</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>729</v>
+      </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I10" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="H15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>352</v>
+      </c>
       <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="H16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>354</v>
+      </c>
       <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="H17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>355</v>
+      </c>
       <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="H18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>359</v>
+      </c>
       <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="H19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>363</v>
+      </c>
       <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="H20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>366</v>
+      </c>
       <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="H21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>381</v>
+      </c>
       <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -4047,12 +4184,182 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4209,7 +4516,7 @@
         <v>38</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -4272,7 +4579,7 @@
         <v>61</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="2"/>
@@ -4924,34 +5231,34 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>241</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>244</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P15" s="7"/>
       <c r="Q15" s="5"/>
@@ -4967,41 +5274,41 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>253</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P16" s="7"/>
       <c r="Q16" s="5"/>
@@ -5017,41 +5324,41 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
@@ -5067,41 +5374,41 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>272</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
@@ -5117,41 +5424,41 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>284</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>290</v>
-      </c>
       <c r="K19" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
@@ -5167,39 +5474,39 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>302</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
@@ -5218,34 +5525,34 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>311</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
@@ -5264,34 +5571,34 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>319</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>320</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
@@ -5310,32 +5617,32 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
@@ -5354,30 +5661,30 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>333</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>335</v>
-      </c>
       <c r="K24" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
@@ -5397,27 +5704,27 @@
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
       <c r="E25" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>347</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
@@ -5437,27 +5744,27 @@
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
@@ -5477,25 +5784,25 @@
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
       <c r="E27" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
@@ -5515,25 +5822,25 @@
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
       <c r="E28" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
@@ -5553,25 +5860,25 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -5591,21 +5898,21 @@
       <c r="C30" s="5"/>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -5627,21 +5934,21 @@
       <c r="C31" s="5"/>
       <c r="D31" s="7"/>
       <c r="E31" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L31" s="5"/>
       <c r="M31" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -5663,21 +5970,21 @@
       <c r="C32" s="5"/>
       <c r="D32" s="7"/>
       <c r="E32" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -5699,21 +6006,21 @@
       <c r="C33" s="5"/>
       <c r="D33" s="7"/>
       <c r="E33" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -5735,21 +6042,21 @@
       <c r="C34" s="5"/>
       <c r="D34" s="7"/>
       <c r="E34" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="N34" s="7"/>
       <c r="O34" s="5"/>
@@ -5771,21 +6078,21 @@
       <c r="C35" s="5"/>
       <c r="D35" s="7"/>
       <c r="E35" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="N35" s="7"/>
       <c r="O35" s="5"/>
@@ -5807,21 +6114,21 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="N36" s="7"/>
       <c r="O36" s="5"/>
@@ -5843,21 +6150,21 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
@@ -5879,21 +6186,21 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
@@ -5915,21 +6222,21 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
@@ -5951,21 +6258,21 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="L40" s="5"/>
       <c r="M40" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
@@ -5987,21 +6294,21 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="L41" s="5"/>
       <c r="M41" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
@@ -6023,21 +6330,21 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
@@ -6059,21 +6366,21 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
@@ -6095,21 +6402,21 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
@@ -6131,21 +6438,21 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="L45" s="5"/>
       <c r="M45" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
@@ -6167,21 +6474,21 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
@@ -6203,21 +6510,21 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L47" s="5"/>
       <c r="M47" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
@@ -6239,21 +6546,21 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
@@ -6275,13 +6582,13 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
@@ -6307,13 +6614,13 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
@@ -6339,13 +6646,13 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
@@ -6371,13 +6678,13 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
@@ -6403,13 +6710,13 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -6435,13 +6742,13 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
@@ -6467,13 +6774,13 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
@@ -6499,13 +6806,13 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
@@ -6531,13 +6838,13 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
@@ -6563,13 +6870,13 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
@@ -6595,13 +6902,13 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
@@ -6627,13 +6934,13 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
@@ -6659,13 +6966,13 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
@@ -6691,13 +6998,13 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
@@ -6723,13 +7030,13 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
@@ -6755,13 +7062,13 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
       <c r="I64" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
@@ -6787,13 +7094,13 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
@@ -6819,13 +7126,13 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
       <c r="I66" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
@@ -6851,13 +7158,13 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
@@ -6883,13 +7190,13 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
       <c r="I68" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
@@ -6915,13 +7222,13 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
@@ -6947,13 +7254,13 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
       <c r="I70" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
@@ -6979,13 +7286,13 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
       <c r="I71" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
@@ -7011,13 +7318,13 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
       <c r="I72" s="5" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
@@ -7043,13 +7350,13 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="5" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
       <c r="I73" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
@@ -7075,13 +7382,13 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
       <c r="I74" s="5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
@@ -7107,13 +7414,13 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="5" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
@@ -7139,13 +7446,13 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
       <c r="I76" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
@@ -7171,13 +7478,13 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
       <c r="I77" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -7203,13 +7510,13 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
       <c r="I78" s="5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
@@ -7235,13 +7542,13 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
       <c r="I79" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
@@ -7267,13 +7574,13 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="I80" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
@@ -7299,13 +7606,13 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
@@ -7331,13 +7638,13 @@
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
       <c r="I82" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
@@ -7363,13 +7670,13 @@
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
       <c r="I83" s="8" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
@@ -7395,13 +7702,13 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
       <c r="I84" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
@@ -7427,13 +7734,13 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="5" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
       <c r="I85" s="5" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
@@ -7459,13 +7766,13 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
       <c r="I86" s="5" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
@@ -7491,13 +7798,13 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="5" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="5" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
@@ -7523,13 +7830,13 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
       <c r="I88" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
@@ -7555,13 +7862,13 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
       <c r="I89" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
@@ -7587,7 +7894,7 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -7617,7 +7924,7 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -7647,7 +7954,7 @@
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
       <c r="E92" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
@@ -7677,7 +7984,7 @@
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
@@ -7707,7 +8014,7 @@
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
@@ -7737,7 +8044,7 @@
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
@@ -7767,7 +8074,7 @@
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
@@ -7797,7 +8104,7 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
@@ -7827,7 +8134,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="5" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
@@ -7857,7 +8164,7 @@
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
       <c r="E99" s="5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
@@ -7887,7 +8194,7 @@
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
@@ -7917,7 +8224,7 @@
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
@@ -7947,7 +8254,7 @@
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
@@ -7977,7 +8284,7 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
@@ -8007,7 +8314,7 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
@@ -8037,7 +8344,7 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
@@ -8067,7 +8374,7 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
@@ -8097,7 +8404,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
@@ -8127,7 +8434,7 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
@@ -8157,7 +8464,7 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
@@ -8187,7 +8494,7 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
@@ -8217,7 +8524,7 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
@@ -8247,7 +8554,7 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="5" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
@@ -8277,7 +8584,7 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
@@ -8307,7 +8614,7 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
@@ -8337,7 +8644,7 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
@@ -8367,7 +8674,7 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="5" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
@@ -8397,7 +8704,7 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="5" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
@@ -8427,7 +8734,7 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="5" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
@@ -8457,7 +8764,7 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="5" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
@@ -8487,7 +8794,7 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
@@ -8517,7 +8824,7 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="5" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
@@ -8547,7 +8854,7 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
@@ -8577,7 +8884,7 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="5" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
@@ -8607,7 +8914,7 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
@@ -8637,7 +8944,7 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="5" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
@@ -8667,7 +8974,7 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="5" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
@@ -8697,7 +9004,7 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
@@ -8727,7 +9034,7 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="5" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
@@ -8757,7 +9064,7 @@
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
@@ -8787,7 +9094,7 @@
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
       <c r="E130" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
@@ -8817,7 +9124,7 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
@@ -8847,7 +9154,7 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
@@ -8877,7 +9184,7 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="5" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
@@ -8907,7 +9214,7 @@
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
@@ -8937,7 +9244,7 @@
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
@@ -8967,7 +9274,7 @@
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
@@ -8997,7 +9304,7 @@
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
@@ -9027,7 +9334,7 @@
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
@@ -9057,7 +9364,7 @@
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
@@ -9087,7 +9394,7 @@
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
@@ -9117,7 +9424,7 @@
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
@@ -9147,7 +9454,7 @@
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
@@ -9177,7 +9484,7 @@
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
@@ -9207,7 +9514,7 @@
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
@@ -9237,7 +9544,7 @@
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
       <c r="E145" s="5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
@@ -9267,7 +9574,7 @@
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
@@ -9297,7 +9604,7 @@
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
@@ -9327,7 +9634,7 @@
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
@@ -9357,7 +9664,7 @@
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
@@ -9387,7 +9694,7 @@
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
       <c r="E150" s="5" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
@@ -9417,7 +9724,7 @@
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
@@ -9447,7 +9754,7 @@
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
@@ -9477,7 +9784,7 @@
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
@@ -9507,7 +9814,7 @@
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
@@ -9537,7 +9844,7 @@
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
@@ -9567,7 +9874,7 @@
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
@@ -9597,7 +9904,7 @@
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
@@ -9627,7 +9934,7 @@
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
       <c r="E158" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
@@ -9657,7 +9964,7 @@
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
@@ -9687,7 +9994,7 @@
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
       <c r="E160" s="5" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
@@ -9717,7 +10024,7 @@
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
@@ -9747,7 +10054,7 @@
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
       <c r="E162" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
@@ -9777,7 +10084,7 @@
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
@@ -9807,7 +10114,7 @@
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
@@ -9837,7 +10144,7 @@
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
@@ -9867,7 +10174,7 @@
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
@@ -9897,7 +10204,7 @@
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
       <c r="E167" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
@@ -9927,7 +10234,7 @@
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
@@ -9957,7 +10264,7 @@
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
       <c r="E169" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
@@ -9987,7 +10294,7 @@
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
@@ -10017,7 +10324,7 @@
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
@@ -10047,7 +10354,7 @@
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
@@ -10077,7 +10384,7 @@
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
       <c r="E173" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
@@ -10107,7 +10414,7 @@
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
@@ -10137,7 +10444,7 @@
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
@@ -10201,8 +10508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10223,153 +10530,153 @@
   <sheetData>
     <row r="1" spans="1:11" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>667</v>
+        <v>730</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>653</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>655</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>657</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -10426,7 +10733,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="22">
@@ -10448,17 +10755,17 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>697</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>698</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>700</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>701</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
@@ -10470,17 +10777,17 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>699</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>699</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>702</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
@@ -10492,7 +10799,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="22"/>
@@ -10508,17 +10815,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="23" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -10530,17 +10837,17 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="23" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
@@ -10552,17 +10859,17 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="23" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
@@ -10574,14 +10881,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="23" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -10594,7 +10901,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
@@ -10610,7 +10917,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>

</xml_diff>